<commit_message>
added base readme, relative links, and excel data validation rules
</commit_message>
<xml_diff>
--- a/resources/seqr_metadata_templates/excel_templates/individuals_metadata_template.xlsx
+++ b/resources/seqr_metadata_templates/excel_templates/individuals_metadata_template.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwfor/Documents/Seqr Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwfor/Code/rare-disease/resources/seqr_metadata_templates/excel_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B4C8BC05-A076-1544-841A-E5A9FB3C5C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E84F0A9-620A-994B-B923-CE8CBBECF7CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5400" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="22820" yWindow="8520" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="individuals_metadata" sheetId="1" r:id="rId1"/>
+    <sheet name="Age of Onset ALLOWED VALUES" sheetId="2" r:id="rId2"/>
+    <sheet name="boolean fields ALLOWED VALUES" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>Family ID</t>
   </si>
@@ -89,13 +91,85 @@
   </si>
   <si>
     <t>Candidate Genes</t>
+  </si>
+  <si>
+    <t>Congenital onset</t>
+  </si>
+  <si>
+    <t>Embryonal onset</t>
+  </si>
+  <si>
+    <t>Fetal onset</t>
+  </si>
+  <si>
+    <t>Neonatal onset</t>
+  </si>
+  <si>
+    <t>Infantile onset</t>
+  </si>
+  <si>
+    <t>Childhood onset</t>
+  </si>
+  <si>
+    <t>Juvenile onset</t>
+  </si>
+  <si>
+    <t>Adult onset</t>
+  </si>
+  <si>
+    <t>Young adult onset</t>
+  </si>
+  <si>
+    <t>Middle age onset</t>
+  </si>
+  <si>
+    <t>Late onset</t>
+  </si>
+  <si>
+    <t>VALUES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Embryonal onset: conception to 8 wks gestation </t>
+  </si>
+  <si>
+    <t>Fetal onset: 9 wks gestation to birth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Congenital onset: conception to birth </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neonatal onset: birth to 1 month, </t>
+  </si>
+  <si>
+    <t>Infantile onset: birth to 1 year</t>
+  </si>
+  <si>
+    <t>Childhood onset: &lt; 5 years</t>
+  </si>
+  <si>
+    <t>Juvenile onset: &lt; 17 years</t>
+  </si>
+  <si>
+    <t>Young adult onset: &lt; 25 years</t>
+  </si>
+  <si>
+    <t>Adult onset: &lt; 36 years</t>
+  </si>
+  <si>
+    <t>Middle age onset: &lt; 55 years</t>
+  </si>
+  <si>
+    <t>Late onset: &gt; 55 years</t>
+  </si>
+  <si>
+    <t>Description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -230,6 +304,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -412,7 +492,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -527,6 +607,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -572,8 +667,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -630,6 +726,27 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7EFDD47B-24F3-AA41-80D8-FC69A9A389A8}" name="Table2" displayName="Table2" ref="A1:B12" totalsRowShown="0">
+  <autoFilter ref="A1:B12" xr:uid="{7EFDD47B-24F3-AA41-80D8-FC69A9A389A8}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{27C0CEBA-1A36-694B-A27F-1FF076A36824}" name="Age of Onset"/>
+    <tableColumn id="2" xr3:uid="{6837260D-03D8-4D4A-8E3F-DF5A72815CFB}" name="Description"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E1CC8383-4451-5745-9B72-10C8DBC1DFFE}" name="Table3" displayName="Table3" ref="A1:A3" totalsRowShown="0">
+  <autoFilter ref="A1:A3" xr:uid="{E1CC8383-4451-5745-9B72-10C8DBC1DFFE}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{B196919C-8A00-AF45-8518-850BCA8A6A12}" name="VALUES"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -928,7 +1045,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1007,6 +1124,181 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576 E2:E1048576" xr:uid="{12AD23A7-D9F6-5A48-8090-4A8C0BDF70BE}">
+      <formula1>1900</formula1>
+      <formula2>2100</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F6D96F51-165E-5641-B1BE-0C33750EAADC}">
+          <x14:formula1>
+            <xm:f>'Age of Onset ALLOWED VALUES'!$A$2:$A$12</xm:f>
+          </x14:formula1>
+          <xm:sqref>G3:G1048576 G2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{34E46654-D885-184F-AC6F-084C535CB411}">
+          <x14:formula1>
+            <xm:f>'boolean fields ALLOWED VALUES'!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>J2:J1048576 L2:L1048576 M2:M1048576 N2:N1048576 O2:O1048576 P2:P1048576 Q2:Q1048576 I2:I1048576 R2:R1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51984378-E1A8-1E4D-A721-AE82D176EF0C}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C84FCF1F-CF6E-7B49-A194-DD00311E38DA}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>